<commit_message>
LED controller done, tone stoppage issue resolved
LED's chage per second now
tone part doens't stop anymore
</commit_message>
<xml_diff>
--- a/lab1_ factor_divider.xlsx
+++ b/lab1_ factor_divider.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melika\Documents\GitHub\CPEN311\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABB843A-DE8A-492E-8B00-F56FDD2CC69F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF789483-EA11-4FBB-B76D-9D8CF0A03EFA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{EE641918-0FE9-42AB-912D-D77D9B10E8DA}"/>
   </bookViews>
@@ -426,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50285A71-9FE1-4F97-9E33-0A3436988C65}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="A1:D11"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,6 +600,18 @@
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>50000000</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" ref="C12" si="1">A12/(B12*2)</f>
+        <v>25000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>